<commit_message>
t test CI works
</commit_message>
<xml_diff>
--- a/regression_t_test.xlsx
+++ b/regression_t_test.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[np.float64(893.6540949337079), np.float64(181.1846868772975)]</t>
+          <t>[np.float64(181.1846868772975), np.float64(893.6540949337079)]</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[np.float64(484.8034289719433), np.float64(-228.5254056673032)]</t>
+          <t>[np.float64(-228.5254056673032), np.float64(484.8034289719433)]</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[np.float64(430.0386702471879), np.float64(388.52208825917734)]</t>
+          <t>[np.float64(388.52208825917734), np.float64(430.0386702471879)]</t>
         </is>
       </c>
     </row>

</xml_diff>